<commit_message>
Upload outputs to GitHub site
</commit_message>
<xml_diff>
--- a/Scenario_comps/Test_EnvDrivers/Fit_metrics_test-STEdrivers.xlsx
+++ b/Scenario_comps/Test_EnvDrivers/Fit_metrics_test-STEdrivers.xlsx
@@ -729,7 +729,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -751,10 +751,10 @@
         <v>4.21</v>
       </c>
       <c r="D7" t="n">
-        <v>2.29</v>
+        <v>2.26</v>
       </c>
       <c r="E7" t="n">
-        <v>12.52</v>
+        <v>12.44</v>
       </c>
       <c r="F7" t="n">
         <v>0.58</v>
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>17.57</v>
+        <v>17.48</v>
       </c>
       <c r="F8" t="n">
         <v>0.99</v>
@@ -806,7 +806,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>17.8</v>
+        <v>17.79</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -855,19 +855,19 @@
         <v>17.16</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E11" t="n">
-        <v>17.05</v>
+        <v>16.35</v>
       </c>
       <c r="F11" t="n">
         <v>0.99</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H11" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="12">
@@ -881,19 +881,19 @@
         <v>13.4</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E12" t="n">
-        <v>13.65</v>
+        <v>14.04</v>
       </c>
       <c r="F12" t="n">
         <v>0.97</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H12" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="13">
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>15.45</v>
+        <v>15.44</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -933,19 +933,19 @@
         <v>11.58</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>10.44</v>
+        <v>11.59</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1014,7 +1014,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>44.2</v>
+        <v>44.27</v>
       </c>
       <c r="F17" t="n">
         <v>3.74</v>
@@ -1037,19 +1037,19 @@
         <v>106.33</v>
       </c>
       <c r="D18" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>91.68</v>
+        <v>106.51</v>
       </c>
       <c r="F18" t="n">
         <v>9.04</v>
       </c>
       <c r="G18" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>8.59</v>
+        <v>9.04</v>
       </c>
     </row>
     <row r="19">
@@ -1063,19 +1063,19 @@
         <v>0.14</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
         <v>0.05</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="H19" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
@@ -1092,13 +1092,13 @@
         <v>0.11</v>
       </c>
       <c r="E20" t="n">
-        <v>179.8</v>
+        <v>177.66</v>
       </c>
       <c r="F20" t="n">
         <v>10.58</v>
       </c>
       <c r="G20" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="H20" t="n">
         <v>10.47</v>
@@ -1118,7 +1118,7 @@
         <v>0.08</v>
       </c>
       <c r="E21" t="n">
-        <v>119.26</v>
+        <v>118.87</v>
       </c>
       <c r="F21" t="n">
         <v>7.64</v>
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>201.18</v>
+        <v>201.06</v>
       </c>
       <c r="F22" t="n">
         <v>12.29</v>
@@ -1167,19 +1167,19 @@
         <v>99.5</v>
       </c>
       <c r="D23" t="n">
-        <v>5.71</v>
+        <v>3.91</v>
       </c>
       <c r="E23" t="n">
-        <v>146.09</v>
+        <v>134.52</v>
       </c>
       <c r="F23" t="n">
         <v>10.67</v>
       </c>
       <c r="G23" t="n">
-        <v>1.65</v>
+        <v>1.35</v>
       </c>
       <c r="H23" t="n">
-        <v>12.63</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="24">
@@ -1196,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>79.29</v>
+        <v>79.24</v>
       </c>
       <c r="F24" t="n">
         <v>5.11</v>
@@ -1219,19 +1219,19 @@
         <v>81.71</v>
       </c>
       <c r="D25" t="n">
-        <v>8.84</v>
+        <v>7.98</v>
       </c>
       <c r="E25" t="n">
-        <v>139.7</v>
+        <v>136.68</v>
       </c>
       <c r="F25" t="n">
         <v>8.19</v>
       </c>
       <c r="G25" t="n">
-        <v>1.83</v>
+        <v>1.72</v>
       </c>
       <c r="H25" t="n">
-        <v>10.13</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="26">
@@ -1245,7 +1245,7 @@
         <v>1.31</v>
       </c>
       <c r="D26" t="n">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="E26" t="n">
         <v>0.05</v>
@@ -1274,7 +1274,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>268.18</v>
+        <v>267.87</v>
       </c>
       <c r="F27" t="n">
         <v>15.32</v>
@@ -1300,7 +1300,7 @@
         <v>0.22</v>
       </c>
       <c r="E28" t="n">
-        <v>365.63</v>
+        <v>364.74</v>
       </c>
       <c r="F28" t="n">
         <v>22.12</v>
@@ -1326,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>71.36</v>
+        <v>71.45</v>
       </c>
       <c r="F29" t="n">
         <v>4.58</v>
@@ -1349,19 +1349,19 @@
         <v>108.01</v>
       </c>
       <c r="D30" t="n">
-        <v>0.36</v>
+        <v>0.14</v>
       </c>
       <c r="E30" t="n">
-        <v>96.95</v>
+        <v>100.56</v>
       </c>
       <c r="F30" t="n">
         <v>7.23</v>
       </c>
       <c r="G30" t="n">
-        <v>0.29</v>
+        <v>0.14</v>
       </c>
       <c r="H30" t="n">
-        <v>7.01</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="31">
@@ -1401,19 +1401,19 @@
         <v>290.78</v>
       </c>
       <c r="D32" t="n">
-        <v>0.21</v>
+        <v>1.24</v>
       </c>
       <c r="E32" t="n">
-        <v>277.53</v>
+        <v>262.41</v>
       </c>
       <c r="F32" t="n">
         <v>20.5</v>
       </c>
       <c r="G32" t="n">
-        <v>0.21</v>
+        <v>0.83</v>
       </c>
       <c r="H32" t="n">
-        <v>20.09</v>
+        <v>19.68</v>
       </c>
     </row>
     <row r="33">
@@ -1475,19 +1475,19 @@
         <v>8.35</v>
       </c>
       <c r="D35" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>7.77</v>
+        <v>8.45</v>
       </c>
       <c r="F35" t="n">
         <v>0.99</v>
       </c>
       <c r="G35" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H35" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="36">
@@ -1527,10 +1527,10 @@
         <v>193.5</v>
       </c>
       <c r="D37" t="n">
-        <v>3.79</v>
+        <v>3.64</v>
       </c>
       <c r="E37" t="n">
-        <v>249.31</v>
+        <v>248.29</v>
       </c>
       <c r="F37" t="n">
         <v>12.97</v>
@@ -1553,19 +1553,19 @@
         <v>209.87</v>
       </c>
       <c r="D38" t="n">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="E38" t="n">
-        <v>204.43</v>
+        <v>215.72</v>
       </c>
       <c r="F38" t="n">
         <v>12.35</v>
       </c>
       <c r="G38" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
       <c r="H38" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
     </row>
     <row r="39">
@@ -1579,19 +1579,19 @@
         <v>270.16</v>
       </c>
       <c r="D39" t="n">
-        <v>5.72</v>
+        <v>5.08</v>
       </c>
       <c r="E39" t="n">
-        <v>345.32</v>
+        <v>341.93</v>
       </c>
       <c r="F39" t="n">
         <v>18.63</v>
       </c>
       <c r="G39" t="n">
-        <v>1.91</v>
+        <v>1.69</v>
       </c>
       <c r="H39" t="n">
-        <v>20.54</v>
+        <v>20.33</v>
       </c>
     </row>
     <row r="40">
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>203.31</v>
+        <v>201.99</v>
       </c>
       <c r="F40" t="n">
         <v>13.17</v>
@@ -1657,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>1.19</v>
+        <v>1.14</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -1679,16 +1679,16 @@
         <v>0.06</v>
       </c>
       <c r="D43" t="n">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="E43" t="n">
-        <v>0.61</v>
+        <v>0.72</v>
       </c>
       <c r="F43" t="n">
         <v>0.06</v>
       </c>
       <c r="G43" t="n">
-        <v>0.22</v>
+        <v>0.28</v>
       </c>
       <c r="H43" t="n">
         <v>0.28</v>
@@ -1705,10 +1705,10 @@
         <v>3.86</v>
       </c>
       <c r="D44" t="n">
-        <v>3.11</v>
+        <v>2.81</v>
       </c>
       <c r="E44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="F44" t="n">
         <v>0.65</v>
@@ -1717,7 +1717,7 @@
         <v>0.56</v>
       </c>
       <c r="H44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45">
@@ -1740,7 +1740,7 @@
         <v>0.14</v>
       </c>
       <c r="G45" t="n">
-        <v>0.43</v>
+        <v>0.29</v>
       </c>
       <c r="H45" t="n">
         <v>0.43</v>
@@ -1757,19 +1757,19 @@
         <v>0.24</v>
       </c>
       <c r="D46" t="n">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F46" t="n">
         <v>0.15</v>
       </c>
       <c r="G46" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="H46" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="47">
@@ -1783,19 +1783,19 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4.24</v>
+        <v>4.7</v>
       </c>
       <c r="E47" t="n">
-        <v>4.43</v>
+        <v>4.98</v>
       </c>
       <c r="F47" t="n">
         <v>0.09</v>
       </c>
       <c r="G47" t="n">
-        <v>1.11</v>
+        <v>1.2</v>
       </c>
       <c r="H47" t="n">
-        <v>1.2</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="48">
@@ -1809,7 +1809,7 @@
         <v>4.36</v>
       </c>
       <c r="D48" t="n">
-        <v>1.37</v>
+        <v>1.42</v>
       </c>
       <c r="E48" t="n">
         <v>2.48</v>
@@ -1835,19 +1835,19 @@
         <v>2.86</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="E49" t="n">
-        <v>2.9</v>
+        <v>2.15</v>
       </c>
       <c r="F49" t="n">
         <v>0.8</v>
       </c>
       <c r="G49" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="H49" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="50">
@@ -1861,19 +1861,19 @@
         <v>3421.7</v>
       </c>
       <c r="D50" t="n">
-        <v>3430.68</v>
+        <v>3343.14</v>
       </c>
       <c r="E50" t="n">
-        <v>2.5</v>
+        <v>6.48</v>
       </c>
       <c r="F50" t="n">
         <v>214.2</v>
       </c>
       <c r="G50" t="n">
-        <v>213.07</v>
+        <v>212.61</v>
       </c>
       <c r="H50" t="n">
-        <v>0.91</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="51">
@@ -1890,16 +1890,16 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>52.9</v>
+        <v>52.75</v>
       </c>
       <c r="F51" t="n">
         <v>3.64</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H51" t="n">
-        <v>3.64</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="52">
@@ -1916,16 +1916,16 @@
         <v>0.06</v>
       </c>
       <c r="E52" t="n">
-        <v>80.48</v>
+        <v>85.77</v>
       </c>
       <c r="F52" t="n">
         <v>5.46</v>
       </c>
       <c r="G52" t="n">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="H52" t="n">
-        <v>5.4</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="53">
@@ -1942,7 +1942,7 @@
         <v>0.21</v>
       </c>
       <c r="E53" t="n">
-        <v>3.53</v>
+        <v>4.47</v>
       </c>
       <c r="F53" t="n">
         <v>1.25</v>
@@ -1951,7 +1951,7 @@
         <v>0.21</v>
       </c>
       <c r="H53" t="n">
-        <v>1.14</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="54">
@@ -1965,14 +1965,14 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="H54"/>
     </row>
@@ -1987,14 +1987,14 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.16</v>
+        <v>0.07</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>0.07</v>
+        <v>0.05</v>
       </c>
       <c r="H55"/>
     </row>
@@ -2031,14 +2031,14 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="H57"/>
     </row>
@@ -2053,19 +2053,19 @@
         <v>19.44</v>
       </c>
       <c r="D58" t="n">
-        <v>0.55</v>
+        <v>0.24</v>
       </c>
       <c r="E58" t="n">
-        <v>24.74</v>
+        <v>21.77</v>
       </c>
       <c r="F58" t="n">
         <v>1.64</v>
       </c>
       <c r="G58" t="n">
-        <v>0.27</v>
+        <v>0.18</v>
       </c>
       <c r="H58" t="n">
-        <v>1.88</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="59">
@@ -2079,19 +2079,19 @@
         <v>6.47</v>
       </c>
       <c r="D59" t="n">
-        <v>3.49</v>
+        <v>5.06</v>
       </c>
       <c r="E59" t="n">
-        <v>12.18</v>
+        <v>16.33</v>
       </c>
       <c r="F59" t="n">
         <v>1.27</v>
       </c>
       <c r="G59" t="n">
-        <v>0.83</v>
+        <v>1.09</v>
       </c>
       <c r="H59" t="n">
-        <v>2.19</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="60">
@@ -2105,19 +2105,19 @@
         <v>602.81</v>
       </c>
       <c r="D60" t="n">
-        <v>46.35</v>
+        <v>64.78</v>
       </c>
       <c r="E60" t="n">
-        <v>851.15</v>
+        <v>941.35</v>
       </c>
       <c r="F60" t="n">
         <v>51.22</v>
       </c>
       <c r="G60" t="n">
-        <v>21.99</v>
+        <v>28.31</v>
       </c>
       <c r="H60" t="n">
-        <v>71.37</v>
+        <v>78.61</v>
       </c>
     </row>
     <row r="61">
@@ -2131,19 +2131,19 @@
         <v>129.96</v>
       </c>
       <c r="D61" t="n">
-        <v>46.22</v>
+        <v>69.66</v>
       </c>
       <c r="E61" t="n">
-        <v>274.54</v>
+        <v>341.7</v>
       </c>
       <c r="F61" t="n">
         <v>15.67</v>
       </c>
       <c r="G61" t="n">
-        <v>12.77</v>
+        <v>17.51</v>
       </c>
       <c r="H61" t="n">
-        <v>28.31</v>
+        <v>33.18</v>
       </c>
     </row>
     <row r="62">
@@ -2160,16 +2160,16 @@
         <v>18.17</v>
       </c>
       <c r="E62" t="n">
-        <v>20.94</v>
+        <v>46.22</v>
       </c>
       <c r="F62" t="n">
         <v>6.98</v>
       </c>
       <c r="G62" t="n">
-        <v>4.61</v>
+        <v>4.74</v>
       </c>
       <c r="H62" t="n">
-        <v>4.48</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="63">
@@ -2183,19 +2183,19 @@
         <v>62.41</v>
       </c>
       <c r="D63" t="n">
-        <v>86.12</v>
+        <v>37.92</v>
       </c>
       <c r="E63" t="n">
-        <v>73.87</v>
+        <v>45.82</v>
       </c>
       <c r="F63" t="n">
         <v>8.16</v>
       </c>
       <c r="G63" t="n">
-        <v>8.82</v>
+        <v>5.79</v>
       </c>
       <c r="H63" t="n">
-        <v>8.03</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="64">
@@ -2209,19 +2209,19 @@
         <v>18.75</v>
       </c>
       <c r="D64" t="n">
-        <v>6.96</v>
+        <v>9.51</v>
       </c>
       <c r="E64" t="n">
-        <v>43.2</v>
+        <v>48.73</v>
       </c>
       <c r="F64" t="n">
         <v>1.53</v>
       </c>
       <c r="G64" t="n">
-        <v>1.04</v>
+        <v>1.26</v>
       </c>
       <c r="H64" t="n">
-        <v>2.6</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="65">
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1.62</v>
+        <v>1.69</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -2257,10 +2257,10 @@
         <v>0.01</v>
       </c>
       <c r="D66" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="E66" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F66" t="n">
         <v>0.01</v>
@@ -2283,19 +2283,19 @@
         <v>165.07</v>
       </c>
       <c r="D67" t="n">
-        <v>29.33</v>
+        <v>38.16</v>
       </c>
       <c r="E67" t="n">
-        <v>72.43</v>
+        <v>56.27</v>
       </c>
       <c r="F67" t="n">
         <v>8.28</v>
       </c>
       <c r="G67" t="n">
-        <v>4.09</v>
+        <v>4.59</v>
       </c>
       <c r="H67" t="n">
-        <v>4.49</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="68">
@@ -2309,19 +2309,19 @@
         <v>208.71</v>
       </c>
       <c r="D68" t="n">
-        <v>3.16</v>
+        <v>2.11</v>
       </c>
       <c r="E68" t="n">
-        <v>163.41</v>
+        <v>171.57</v>
       </c>
       <c r="F68" t="n">
         <v>13.17</v>
       </c>
       <c r="G68" t="n">
-        <v>1.05</v>
+        <v>0.92</v>
       </c>
       <c r="H68" t="n">
-        <v>11.98</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="69">
@@ -2335,19 +2335,19 @@
         <v>211.73</v>
       </c>
       <c r="D69" t="n">
-        <v>1.98</v>
+        <v>0.66</v>
       </c>
       <c r="E69" t="n">
-        <v>175.65</v>
+        <v>192.38</v>
       </c>
       <c r="F69" t="n">
         <v>13.17</v>
       </c>
       <c r="G69" t="n">
-        <v>0.79</v>
+        <v>0.4</v>
       </c>
       <c r="H69" t="n">
-        <v>12.38</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="70">
@@ -2361,19 +2361,19 @@
         <v>157.48</v>
       </c>
       <c r="D70" t="n">
-        <v>47.4</v>
+        <v>43.19</v>
       </c>
       <c r="E70" t="n">
-        <v>48.32</v>
+        <v>50.96</v>
       </c>
       <c r="F70" t="n">
         <v>11.59</v>
       </c>
       <c r="G70" t="n">
-        <v>5.27</v>
+        <v>5</v>
       </c>
       <c r="H70" t="n">
-        <v>6.32</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="71">
@@ -2387,19 +2387,19 @@
         <v>0.29</v>
       </c>
       <c r="D71" t="n">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="E71" t="n">
-        <v>0.19</v>
+        <v>0.77</v>
       </c>
       <c r="F71" t="n">
         <v>0.07</v>
       </c>
       <c r="G71" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="H71" t="n">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="72">
@@ -2413,14 +2413,14 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>74.01</v>
+        <v>65.45</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>34.38</v>
+        <v>33.34</v>
       </c>
       <c r="H72"/>
     </row>
@@ -2435,19 +2435,19 @@
         <v>92.44</v>
       </c>
       <c r="D73" t="n">
-        <v>19.01</v>
+        <v>19.08</v>
       </c>
       <c r="E73" t="n">
-        <v>191.96</v>
+        <v>192.18</v>
       </c>
       <c r="F73" t="n">
         <v>4.32</v>
       </c>
       <c r="G73" t="n">
-        <v>7.28</v>
+        <v>7.3</v>
       </c>
       <c r="H73" t="n">
-        <v>11.65</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="74">
@@ -2461,14 +2461,14 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>2.28</v>
+        <v>2.85</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>2.98</v>
+        <v>3.12</v>
       </c>
       <c r="H74"/>
     </row>
@@ -2483,14 +2483,14 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>1.48</v>
+        <v>1.47</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>3.39</v>
+        <v>3.38</v>
       </c>
       <c r="H75"/>
     </row>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>4.58</v>
+        <v>4.6</v>
       </c>
       <c r="H76"/>
     </row>
@@ -2527,14 +2527,14 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>363.38</v>
+        <v>359.75</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>121.71</v>
+        <v>119.73</v>
       </c>
       <c r="H77"/>
     </row>
@@ -2549,14 +2549,14 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.61</v>
+        <v>0.68</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>3.05</v>
+        <v>3.27</v>
       </c>
       <c r="H78"/>
     </row>
@@ -2571,14 +2571,14 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>11.34</v>
+        <v>11.25</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>41.73</v>
+        <v>41.51</v>
       </c>
       <c r="H79"/>
     </row>
@@ -2721,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -2743,10 +2743,10 @@
         <v>4.19</v>
       </c>
       <c r="D7" t="n">
-        <v>2.32</v>
+        <v>2.29</v>
       </c>
       <c r="E7" t="n">
-        <v>12.52</v>
+        <v>12.44</v>
       </c>
       <c r="F7" t="n">
         <v>0.58</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>17.57</v>
+        <v>17.48</v>
       </c>
       <c r="F8" t="n">
         <v>0.99</v>
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>17.8</v>
+        <v>17.79</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -2847,19 +2847,19 @@
         <v>17.18</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E11" t="n">
-        <v>17.05</v>
+        <v>16.35</v>
       </c>
       <c r="F11" t="n">
         <v>0.99</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H11" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="12">
@@ -2873,19 +2873,19 @@
         <v>13.39</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E12" t="n">
-        <v>13.65</v>
+        <v>14.04</v>
       </c>
       <c r="F12" t="n">
         <v>0.97</v>
       </c>
       <c r="G12" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H12" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="13">
@@ -2902,7 +2902,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>15.45</v>
+        <v>15.44</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -2925,19 +2925,19 @@
         <v>11.58</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>10.44</v>
+        <v>11.59</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -3006,7 +3006,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>44.2</v>
+        <v>44.27</v>
       </c>
       <c r="F17" t="n">
         <v>3.74</v>
@@ -3029,19 +3029,19 @@
         <v>106.33</v>
       </c>
       <c r="D18" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>91.68</v>
+        <v>106.51</v>
       </c>
       <c r="F18" t="n">
         <v>9.04</v>
       </c>
       <c r="G18" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>8.59</v>
+        <v>9.04</v>
       </c>
     </row>
     <row r="19">
@@ -3055,19 +3055,19 @@
         <v>0.14</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
         <v>0.05</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="H19" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
@@ -3084,13 +3084,13 @@
         <v>0.11</v>
       </c>
       <c r="E20" t="n">
-        <v>179.8</v>
+        <v>177.66</v>
       </c>
       <c r="F20" t="n">
         <v>10.58</v>
       </c>
       <c r="G20" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="H20" t="n">
         <v>10.47</v>
@@ -3110,7 +3110,7 @@
         <v>0.08</v>
       </c>
       <c r="E21" t="n">
-        <v>119.26</v>
+        <v>118.87</v>
       </c>
       <c r="F21" t="n">
         <v>7.64</v>
@@ -3136,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>201.18</v>
+        <v>201.06</v>
       </c>
       <c r="F22" t="n">
         <v>12.29</v>
@@ -3159,19 +3159,19 @@
         <v>101.75</v>
       </c>
       <c r="D23" t="n">
-        <v>5.26</v>
+        <v>3.76</v>
       </c>
       <c r="E23" t="n">
-        <v>146.09</v>
+        <v>134.52</v>
       </c>
       <c r="F23" t="n">
         <v>10.82</v>
       </c>
       <c r="G23" t="n">
-        <v>1.65</v>
+        <v>1.35</v>
       </c>
       <c r="H23" t="n">
-        <v>12.63</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="24">
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>79.29</v>
+        <v>79.24</v>
       </c>
       <c r="F24" t="n">
         <v>5.11</v>
@@ -3211,19 +3211,19 @@
         <v>82.57</v>
       </c>
       <c r="D25" t="n">
-        <v>8.62</v>
+        <v>7.76</v>
       </c>
       <c r="E25" t="n">
-        <v>139.7</v>
+        <v>136.68</v>
       </c>
       <c r="F25" t="n">
         <v>8.3</v>
       </c>
       <c r="G25" t="n">
-        <v>1.83</v>
+        <v>1.72</v>
       </c>
       <c r="H25" t="n">
-        <v>10.13</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="26">
@@ -3237,7 +3237,7 @@
         <v>1.28</v>
       </c>
       <c r="D26" t="n">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="E26" t="n">
         <v>0.05</v>
@@ -3266,7 +3266,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>268.18</v>
+        <v>267.87</v>
       </c>
       <c r="F27" t="n">
         <v>15.32</v>
@@ -3292,7 +3292,7 @@
         <v>0.22</v>
       </c>
       <c r="E28" t="n">
-        <v>365.63</v>
+        <v>364.74</v>
       </c>
       <c r="F28" t="n">
         <v>22.12</v>
@@ -3318,7 +3318,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>71.36</v>
+        <v>71.45</v>
       </c>
       <c r="F29" t="n">
         <v>4.58</v>
@@ -3341,19 +3341,19 @@
         <v>108.01</v>
       </c>
       <c r="D30" t="n">
-        <v>0.36</v>
+        <v>0.14</v>
       </c>
       <c r="E30" t="n">
-        <v>96.95</v>
+        <v>100.56</v>
       </c>
       <c r="F30" t="n">
         <v>7.23</v>
       </c>
       <c r="G30" t="n">
-        <v>0.29</v>
+        <v>0.14</v>
       </c>
       <c r="H30" t="n">
-        <v>7.01</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="31">
@@ -3393,19 +3393,19 @@
         <v>289.96</v>
       </c>
       <c r="D32" t="n">
-        <v>0.21</v>
+        <v>1.24</v>
       </c>
       <c r="E32" t="n">
-        <v>277.53</v>
+        <v>262.41</v>
       </c>
       <c r="F32" t="n">
         <v>20.5</v>
       </c>
       <c r="G32" t="n">
-        <v>0.21</v>
+        <v>0.83</v>
       </c>
       <c r="H32" t="n">
-        <v>20.09</v>
+        <v>19.68</v>
       </c>
     </row>
     <row r="33">
@@ -3467,19 +3467,19 @@
         <v>8.34</v>
       </c>
       <c r="D35" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>7.77</v>
+        <v>8.45</v>
       </c>
       <c r="F35" t="n">
         <v>0.99</v>
       </c>
       <c r="G35" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H35" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="36">
@@ -3522,13 +3522,13 @@
         <v>3.5</v>
       </c>
       <c r="E37" t="n">
-        <v>249.31</v>
+        <v>248.29</v>
       </c>
       <c r="F37" t="n">
         <v>12.97</v>
       </c>
       <c r="G37" t="n">
-        <v>1.31</v>
+        <v>1.17</v>
       </c>
       <c r="H37" t="n">
         <v>14.28</v>
@@ -3545,19 +3545,19 @@
         <v>210.27</v>
       </c>
       <c r="D38" t="n">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="E38" t="n">
-        <v>204.43</v>
+        <v>215.72</v>
       </c>
       <c r="F38" t="n">
         <v>12.48</v>
       </c>
       <c r="G38" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
       <c r="H38" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
     </row>
     <row r="39">
@@ -3571,10 +3571,10 @@
         <v>274.6</v>
       </c>
       <c r="D39" t="n">
-        <v>5.08</v>
+        <v>4.45</v>
       </c>
       <c r="E39" t="n">
-        <v>345.32</v>
+        <v>341.93</v>
       </c>
       <c r="F39" t="n">
         <v>18.63</v>
@@ -3583,7 +3583,7 @@
         <v>1.69</v>
       </c>
       <c r="H39" t="n">
-        <v>20.54</v>
+        <v>20.33</v>
       </c>
     </row>
     <row r="40">
@@ -3600,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>203.31</v>
+        <v>201.99</v>
       </c>
       <c r="F40" t="n">
         <v>13.17</v>
@@ -3649,14 +3649,14 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="H42"/>
     </row>
@@ -3671,16 +3671,16 @@
         <v>0.06</v>
       </c>
       <c r="D43" t="n">
-        <v>0.45</v>
+        <v>0.56</v>
       </c>
       <c r="E43" t="n">
-        <v>0.61</v>
+        <v>0.72</v>
       </c>
       <c r="F43" t="n">
         <v>0.06</v>
       </c>
       <c r="G43" t="n">
-        <v>0.22</v>
+        <v>0.28</v>
       </c>
       <c r="H43" t="n">
         <v>0.28</v>
@@ -3697,19 +3697,19 @@
         <v>3.93</v>
       </c>
       <c r="D44" t="n">
-        <v>3.17</v>
+        <v>2.85</v>
       </c>
       <c r="E44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="F44" t="n">
         <v>0.65</v>
       </c>
       <c r="G44" t="n">
-        <v>0.59</v>
+        <v>0.56</v>
       </c>
       <c r="H44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45">
@@ -3732,7 +3732,7 @@
         <v>0.14</v>
       </c>
       <c r="G45" t="n">
-        <v>0.43</v>
+        <v>0.29</v>
       </c>
       <c r="H45" t="n">
         <v>0.43</v>
@@ -3749,19 +3749,19 @@
         <v>0.24</v>
       </c>
       <c r="D46" t="n">
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F46" t="n">
         <v>0.15</v>
       </c>
       <c r="G46" t="n">
-        <v>0.12</v>
+        <v>0.09</v>
       </c>
       <c r="H46" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="47">
@@ -3775,19 +3775,19 @@
         <v>0.09</v>
       </c>
       <c r="D47" t="n">
-        <v>4.15</v>
+        <v>4.7</v>
       </c>
       <c r="E47" t="n">
-        <v>4.43</v>
+        <v>4.98</v>
       </c>
       <c r="F47" t="n">
         <v>0.09</v>
       </c>
       <c r="G47" t="n">
-        <v>1.11</v>
+        <v>1.2</v>
       </c>
       <c r="H47" t="n">
-        <v>1.2</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="48">
@@ -3827,19 +3827,19 @@
         <v>2.89</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03</v>
+        <v>0.14</v>
       </c>
       <c r="E49" t="n">
-        <v>2.9</v>
+        <v>2.15</v>
       </c>
       <c r="F49" t="n">
         <v>0.8</v>
       </c>
       <c r="G49" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="H49" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="50">
@@ -3853,19 +3853,19 @@
         <v>3369.63</v>
       </c>
       <c r="D50" t="n">
-        <v>3381</v>
+        <v>3294.93</v>
       </c>
       <c r="E50" t="n">
-        <v>2.5</v>
+        <v>6.48</v>
       </c>
       <c r="F50" t="n">
         <v>209.32</v>
       </c>
       <c r="G50" t="n">
-        <v>208.52</v>
+        <v>208.06</v>
       </c>
       <c r="H50" t="n">
-        <v>0.91</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="51">
@@ -3882,16 +3882,16 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>52.9</v>
+        <v>52.75</v>
       </c>
       <c r="F51" t="n">
         <v>3.64</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H51" t="n">
-        <v>3.64</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="52">
@@ -3908,16 +3908,16 @@
         <v>0.06</v>
       </c>
       <c r="E52" t="n">
-        <v>80.48</v>
+        <v>85.77</v>
       </c>
       <c r="F52" t="n">
         <v>5.46</v>
       </c>
       <c r="G52" t="n">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="H52" t="n">
-        <v>5.4</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="53">
@@ -3931,19 +3931,19 @@
         <v>5.19</v>
       </c>
       <c r="D53" t="n">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="E53" t="n">
-        <v>3.53</v>
+        <v>4.47</v>
       </c>
       <c r="F53" t="n">
         <v>1.35</v>
       </c>
       <c r="G53" t="n">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="H53" t="n">
-        <v>1.14</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="54">
@@ -3957,14 +3957,14 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.07</v>
+        <v>0.04</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H54"/>
     </row>
@@ -3979,14 +3979,14 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.15</v>
+        <v>0.07</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>0.07</v>
+        <v>0.05</v>
       </c>
       <c r="H55"/>
     </row>
@@ -4023,14 +4023,14 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="H57"/>
     </row>
@@ -4045,19 +4045,19 @@
         <v>19.11</v>
       </c>
       <c r="D58" t="n">
-        <v>0.64</v>
+        <v>0.3</v>
       </c>
       <c r="E58" t="n">
-        <v>24.74</v>
+        <v>21.77</v>
       </c>
       <c r="F58" t="n">
         <v>1.6</v>
       </c>
       <c r="G58" t="n">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="H58" t="n">
-        <v>1.88</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="59">
@@ -4071,19 +4071,19 @@
         <v>5.98</v>
       </c>
       <c r="D59" t="n">
-        <v>4.02</v>
+        <v>5.74</v>
       </c>
       <c r="E59" t="n">
-        <v>12.18</v>
+        <v>16.33</v>
       </c>
       <c r="F59" t="n">
         <v>1.18</v>
       </c>
       <c r="G59" t="n">
-        <v>0.88</v>
+        <v>1.15</v>
       </c>
       <c r="H59" t="n">
-        <v>2.19</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="60">
@@ -4097,19 +4097,19 @@
         <v>569.1</v>
       </c>
       <c r="D60" t="n">
-        <v>54.78</v>
+        <v>75.32</v>
       </c>
       <c r="E60" t="n">
-        <v>851.15</v>
+        <v>941.35</v>
       </c>
       <c r="F60" t="n">
         <v>48.85</v>
       </c>
       <c r="G60" t="n">
-        <v>23.7</v>
+        <v>30.42</v>
       </c>
       <c r="H60" t="n">
-        <v>71.37</v>
+        <v>78.61</v>
       </c>
     </row>
     <row r="61">
@@ -4123,19 +4123,19 @@
         <v>119.56</v>
       </c>
       <c r="D61" t="n">
-        <v>52.67</v>
+        <v>77.95</v>
       </c>
       <c r="E61" t="n">
-        <v>274.54</v>
+        <v>341.7</v>
       </c>
       <c r="F61" t="n">
         <v>14.75</v>
       </c>
       <c r="G61" t="n">
-        <v>13.56</v>
+        <v>18.43</v>
       </c>
       <c r="H61" t="n">
-        <v>28.31</v>
+        <v>33.18</v>
       </c>
     </row>
     <row r="62">
@@ -4149,19 +4149,19 @@
         <v>43.72</v>
       </c>
       <c r="D62" t="n">
-        <v>16.85</v>
+        <v>19.36</v>
       </c>
       <c r="E62" t="n">
-        <v>20.94</v>
+        <v>46.22</v>
       </c>
       <c r="F62" t="n">
         <v>6.72</v>
       </c>
       <c r="G62" t="n">
-        <v>4.48</v>
+        <v>4.74</v>
       </c>
       <c r="H62" t="n">
-        <v>4.48</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="63">
@@ -4175,19 +4175,19 @@
         <v>60.18</v>
       </c>
       <c r="D63" t="n">
-        <v>78.74</v>
+        <v>33.71</v>
       </c>
       <c r="E63" t="n">
-        <v>73.87</v>
+        <v>45.82</v>
       </c>
       <c r="F63" t="n">
         <v>8.03</v>
       </c>
       <c r="G63" t="n">
-        <v>8.3</v>
+        <v>5.4</v>
       </c>
       <c r="H63" t="n">
-        <v>8.03</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="64">
@@ -4201,19 +4201,19 @@
         <v>16.97</v>
       </c>
       <c r="D64" t="n">
-        <v>8.28</v>
+        <v>11.05</v>
       </c>
       <c r="E64" t="n">
-        <v>43.2</v>
+        <v>48.73</v>
       </c>
       <c r="F64" t="n">
         <v>1.43</v>
       </c>
       <c r="G64" t="n">
-        <v>1.15</v>
+        <v>1.34</v>
       </c>
       <c r="H64" t="n">
-        <v>2.6</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="65">
@@ -4227,7 +4227,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1.62</v>
+        <v>1.69</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -4249,10 +4249,10 @@
         <v>0.01</v>
       </c>
       <c r="D66" t="n">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="E66" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F66" t="n">
         <v>0.01</v>
@@ -4275,19 +4275,19 @@
         <v>175.65</v>
       </c>
       <c r="D67" t="n">
-        <v>32.28</v>
+        <v>42.1</v>
       </c>
       <c r="E67" t="n">
-        <v>72.43</v>
+        <v>56.27</v>
       </c>
       <c r="F67" t="n">
         <v>8.68</v>
       </c>
       <c r="G67" t="n">
-        <v>4.34</v>
+        <v>4.84</v>
       </c>
       <c r="H67" t="n">
-        <v>4.49</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="68">
@@ -4301,19 +4301,19 @@
         <v>208.84</v>
       </c>
       <c r="D68" t="n">
-        <v>3.29</v>
+        <v>2.11</v>
       </c>
       <c r="E68" t="n">
-        <v>163.41</v>
+        <v>171.57</v>
       </c>
       <c r="F68" t="n">
         <v>13.17</v>
       </c>
       <c r="G68" t="n">
-        <v>1.05</v>
+        <v>0.92</v>
       </c>
       <c r="H68" t="n">
-        <v>11.98</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="69">
@@ -4327,19 +4327,19 @@
         <v>211.73</v>
       </c>
       <c r="D69" t="n">
-        <v>1.98</v>
+        <v>0.66</v>
       </c>
       <c r="E69" t="n">
-        <v>175.65</v>
+        <v>192.38</v>
       </c>
       <c r="F69" t="n">
         <v>13.17</v>
       </c>
       <c r="G69" t="n">
-        <v>0.79</v>
+        <v>0.4</v>
       </c>
       <c r="H69" t="n">
-        <v>12.38</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="70">
@@ -4353,19 +4353,19 @@
         <v>157.35</v>
       </c>
       <c r="D70" t="n">
-        <v>47.53</v>
+        <v>43.32</v>
       </c>
       <c r="E70" t="n">
-        <v>48.32</v>
+        <v>50.96</v>
       </c>
       <c r="F70" t="n">
         <v>11.59</v>
       </c>
       <c r="G70" t="n">
-        <v>5.27</v>
+        <v>5</v>
       </c>
       <c r="H70" t="n">
-        <v>6.32</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="71">
@@ -4379,19 +4379,19 @@
         <v>0.3</v>
       </c>
       <c r="D71" t="n">
-        <v>0.03</v>
+        <v>0.13</v>
       </c>
       <c r="E71" t="n">
-        <v>0.19</v>
+        <v>0.77</v>
       </c>
       <c r="F71" t="n">
         <v>0.07</v>
       </c>
       <c r="G71" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="H71" t="n">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="72">
@@ -4405,14 +4405,14 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>71.81</v>
+        <v>63.46</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>33.19</v>
+        <v>32.15</v>
       </c>
       <c r="H72"/>
     </row>
@@ -4427,19 +4427,19 @@
         <v>91.73</v>
       </c>
       <c r="D73" t="n">
-        <v>19.48</v>
+        <v>19.55</v>
       </c>
       <c r="E73" t="n">
-        <v>191.96</v>
+        <v>192.18</v>
       </c>
       <c r="F73" t="n">
         <v>4.28</v>
       </c>
       <c r="G73" t="n">
-        <v>7.32</v>
+        <v>7.33</v>
       </c>
       <c r="H73" t="n">
-        <v>11.65</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="74">
@@ -4453,14 +4453,14 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>2.19</v>
+        <v>2.93</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>2.95</v>
+        <v>3.14</v>
       </c>
       <c r="H74"/>
     </row>
@@ -4482,7 +4482,7 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>3.34</v>
+        <v>3.33</v>
       </c>
       <c r="H75"/>
     </row>
@@ -4504,7 +4504,7 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>4.57</v>
+        <v>4.59</v>
       </c>
       <c r="H76"/>
     </row>
@@ -4519,14 +4519,14 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>364.44</v>
+        <v>360.8</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>121.74</v>
+        <v>119.75</v>
       </c>
       <c r="H77"/>
     </row>
@@ -4541,14 +4541,14 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.6</v>
+        <v>0.66</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>3.02</v>
+        <v>3.24</v>
       </c>
       <c r="H78"/>
     </row>
@@ -4563,14 +4563,14 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>11.28</v>
+        <v>11.19</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>41.65</v>
+        <v>41.44</v>
       </c>
       <c r="H79"/>
     </row>
@@ -4647,7 +4647,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -4735,16 +4735,16 @@
         <v>7.3</v>
       </c>
       <c r="D7" t="n">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="E7" t="n">
-        <v>12.52</v>
+        <v>12.44</v>
       </c>
       <c r="F7" t="n">
         <v>0.72</v>
       </c>
       <c r="G7" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="H7" t="n">
         <v>0.89</v>
@@ -4764,7 +4764,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>17.57</v>
+        <v>17.48</v>
       </c>
       <c r="F8" t="n">
         <v>0.99</v>
@@ -4790,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>17.8</v>
+        <v>17.79</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -4839,19 +4839,19 @@
         <v>17.07</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E11" t="n">
-        <v>17.05</v>
+        <v>16.35</v>
       </c>
       <c r="F11" t="n">
         <v>0.99</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H11" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="12">
@@ -4868,7 +4868,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>13.65</v>
+        <v>14.04</v>
       </c>
       <c r="F12" t="n">
         <v>0.98</v>
@@ -4877,7 +4877,7 @@
         <v>0.01</v>
       </c>
       <c r="H12" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="13">
@@ -4894,7 +4894,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>15.45</v>
+        <v>15.44</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -4917,19 +4917,19 @@
         <v>11.58</v>
       </c>
       <c r="D14" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>10.44</v>
+        <v>11.59</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -4998,7 +4998,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>44.2</v>
+        <v>44.27</v>
       </c>
       <c r="F17" t="n">
         <v>3.74</v>
@@ -5021,19 +5021,19 @@
         <v>106.33</v>
       </c>
       <c r="D18" t="n">
-        <v>0.72</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>91.68</v>
+        <v>106.51</v>
       </c>
       <c r="F18" t="n">
         <v>9.04</v>
       </c>
       <c r="G18" t="n">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>8.59</v>
+        <v>9.04</v>
       </c>
     </row>
     <row r="19">
@@ -5050,7 +5050,7 @@
         <v>0.01</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
         <v>0.03</v>
@@ -5059,7 +5059,7 @@
         <v>0.01</v>
       </c>
       <c r="H19" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
@@ -5076,13 +5076,13 @@
         <v>0.11</v>
       </c>
       <c r="E20" t="n">
-        <v>179.8</v>
+        <v>177.66</v>
       </c>
       <c r="F20" t="n">
         <v>10.58</v>
       </c>
       <c r="G20" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="H20" t="n">
         <v>10.47</v>
@@ -5102,7 +5102,7 @@
         <v>0.08</v>
       </c>
       <c r="E21" t="n">
-        <v>119.26</v>
+        <v>118.87</v>
       </c>
       <c r="F21" t="n">
         <v>7.64</v>
@@ -5128,7 +5128,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>201.18</v>
+        <v>201.06</v>
       </c>
       <c r="F22" t="n">
         <v>12.29</v>
@@ -5151,19 +5151,19 @@
         <v>114.83</v>
       </c>
       <c r="D23" t="n">
-        <v>2.71</v>
+        <v>1.8</v>
       </c>
       <c r="E23" t="n">
-        <v>146.09</v>
+        <v>134.52</v>
       </c>
       <c r="F23" t="n">
         <v>11.27</v>
       </c>
       <c r="G23" t="n">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="H23" t="n">
-        <v>12.63</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="24">
@@ -5180,7 +5180,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>79.29</v>
+        <v>79.24</v>
       </c>
       <c r="F24" t="n">
         <v>5.11</v>
@@ -5203,19 +5203,19 @@
         <v>107.47</v>
       </c>
       <c r="D25" t="n">
-        <v>2.37</v>
+        <v>2.05</v>
       </c>
       <c r="E25" t="n">
-        <v>139.7</v>
+        <v>136.68</v>
       </c>
       <c r="F25" t="n">
         <v>9.16</v>
       </c>
       <c r="G25" t="n">
-        <v>0.86</v>
+        <v>0.75</v>
       </c>
       <c r="H25" t="n">
-        <v>10.13</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="26">
@@ -5258,7 +5258,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>268.18</v>
+        <v>267.87</v>
       </c>
       <c r="F27" t="n">
         <v>15.32</v>
@@ -5284,7 +5284,7 @@
         <v>0.22</v>
       </c>
       <c r="E28" t="n">
-        <v>365.63</v>
+        <v>364.74</v>
       </c>
       <c r="F28" t="n">
         <v>22.12</v>
@@ -5310,7 +5310,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>71.36</v>
+        <v>71.45</v>
       </c>
       <c r="F29" t="n">
         <v>4.58</v>
@@ -5333,19 +5333,19 @@
         <v>108.3</v>
       </c>
       <c r="D30" t="n">
-        <v>0.36</v>
+        <v>0.14</v>
       </c>
       <c r="E30" t="n">
-        <v>96.95</v>
+        <v>100.56</v>
       </c>
       <c r="F30" t="n">
         <v>7.23</v>
       </c>
       <c r="G30" t="n">
-        <v>0.29</v>
+        <v>0.22</v>
       </c>
       <c r="H30" t="n">
-        <v>7.01</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="31">
@@ -5385,19 +5385,19 @@
         <v>289.96</v>
       </c>
       <c r="D32" t="n">
-        <v>0.21</v>
+        <v>1.24</v>
       </c>
       <c r="E32" t="n">
-        <v>277.53</v>
+        <v>262.41</v>
       </c>
       <c r="F32" t="n">
         <v>20.5</v>
       </c>
       <c r="G32" t="n">
-        <v>0.21</v>
+        <v>0.83</v>
       </c>
       <c r="H32" t="n">
-        <v>20.09</v>
+        <v>19.68</v>
       </c>
     </row>
     <row r="33">
@@ -5459,19 +5459,19 @@
         <v>7.82</v>
       </c>
       <c r="D35" t="n">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="E35" t="n">
-        <v>7.77</v>
+        <v>8.45</v>
       </c>
       <c r="F35" t="n">
         <v>0.96</v>
       </c>
       <c r="G35" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="H35" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="36">
@@ -5514,7 +5514,7 @@
         <v>0.29</v>
       </c>
       <c r="E37" t="n">
-        <v>249.31</v>
+        <v>248.29</v>
       </c>
       <c r="F37" t="n">
         <v>13.99</v>
@@ -5537,19 +5537,19 @@
         <v>229.65</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8</v>
+        <v>0.27</v>
       </c>
       <c r="E38" t="n">
-        <v>204.43</v>
+        <v>215.72</v>
       </c>
       <c r="F38" t="n">
         <v>12.88</v>
       </c>
       <c r="G38" t="n">
-        <v>0.4</v>
+        <v>0.27</v>
       </c>
       <c r="H38" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
     </row>
     <row r="39">
@@ -5563,19 +5563,19 @@
         <v>280.11</v>
       </c>
       <c r="D39" t="n">
-        <v>4.45</v>
+        <v>3.81</v>
       </c>
       <c r="E39" t="n">
-        <v>345.32</v>
+        <v>341.93</v>
       </c>
       <c r="F39" t="n">
         <v>18.84</v>
       </c>
       <c r="G39" t="n">
-        <v>1.69</v>
+        <v>1.48</v>
       </c>
       <c r="H39" t="n">
-        <v>20.54</v>
+        <v>20.33</v>
       </c>
     </row>
     <row r="40">
@@ -5592,7 +5592,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>203.31</v>
+        <v>201.99</v>
       </c>
       <c r="F40" t="n">
         <v>13.17</v>
@@ -5641,14 +5641,14 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>1.06</v>
+        <v>1.01</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="H42"/>
     </row>
@@ -5663,10 +5663,10 @@
         <v>0.11</v>
       </c>
       <c r="D43" t="n">
-        <v>0.95</v>
+        <v>1.06</v>
       </c>
       <c r="E43" t="n">
-        <v>0.61</v>
+        <v>0.72</v>
       </c>
       <c r="F43" t="n">
         <v>0.11</v>
@@ -5689,19 +5689,19 @@
         <v>6.22</v>
       </c>
       <c r="D44" t="n">
-        <v>5.3</v>
+        <v>4.91</v>
       </c>
       <c r="E44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="F44" t="n">
         <v>0.85</v>
       </c>
       <c r="G44" t="n">
-        <v>0.79</v>
+        <v>0.75</v>
       </c>
       <c r="H44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45">
@@ -5741,19 +5741,19 @@
         <v>0.18</v>
       </c>
       <c r="D46" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F46" t="n">
         <v>0.12</v>
       </c>
       <c r="G46" t="n">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="H46" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="47">
@@ -5767,19 +5767,19 @@
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>4.24</v>
+        <v>4.7</v>
       </c>
       <c r="E47" t="n">
-        <v>4.43</v>
+        <v>4.98</v>
       </c>
       <c r="F47" t="n">
         <v>0.09</v>
       </c>
       <c r="G47" t="n">
-        <v>1.11</v>
+        <v>1.2</v>
       </c>
       <c r="H47" t="n">
-        <v>1.2</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="48">
@@ -5819,19 +5819,19 @@
         <v>2.95</v>
       </c>
       <c r="D49" t="n">
-        <v>0.04</v>
+        <v>0.18</v>
       </c>
       <c r="E49" t="n">
-        <v>2.9</v>
+        <v>2.15</v>
       </c>
       <c r="F49" t="n">
         <v>0.81</v>
       </c>
       <c r="G49" t="n">
-        <v>0.03</v>
+        <v>0.07</v>
       </c>
       <c r="H49" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="50">
@@ -5845,19 +5845,19 @@
         <v>2225.84</v>
       </c>
       <c r="D50" t="n">
-        <v>2202.65</v>
+        <v>2132.84</v>
       </c>
       <c r="E50" t="n">
-        <v>2.5</v>
+        <v>6.48</v>
       </c>
       <c r="F50" t="n">
         <v>116.2</v>
       </c>
       <c r="G50" t="n">
-        <v>115.17</v>
+        <v>114.61</v>
       </c>
       <c r="H50" t="n">
-        <v>0.91</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="51">
@@ -5874,7 +5874,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>52.9</v>
+        <v>52.75</v>
       </c>
       <c r="F51" t="n">
         <v>3.64</v>
@@ -5883,7 +5883,7 @@
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>3.64</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="52">
@@ -5897,19 +5897,19 @@
         <v>87.84</v>
       </c>
       <c r="D52" t="n">
-        <v>0.23</v>
+        <v>0.06</v>
       </c>
       <c r="E52" t="n">
-        <v>80.48</v>
+        <v>85.77</v>
       </c>
       <c r="F52" t="n">
         <v>5.57</v>
       </c>
       <c r="G52" t="n">
-        <v>0.17</v>
+        <v>0.06</v>
       </c>
       <c r="H52" t="n">
-        <v>5.4</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="53">
@@ -5923,19 +5923,19 @@
         <v>5.61</v>
       </c>
       <c r="D53" t="n">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="E53" t="n">
-        <v>3.53</v>
+        <v>4.47</v>
       </c>
       <c r="F53" t="n">
         <v>1.45</v>
       </c>
       <c r="G53" t="n">
-        <v>0.31</v>
+        <v>0.21</v>
       </c>
       <c r="H53" t="n">
-        <v>1.14</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="54">
@@ -5949,14 +5949,14 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.36</v>
+        <v>0.29</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H54"/>
     </row>
@@ -5971,14 +5971,14 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="H55"/>
     </row>
@@ -6015,14 +6015,14 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="H57"/>
     </row>
@@ -6037,19 +6037,19 @@
         <v>20.35</v>
       </c>
       <c r="D58" t="n">
-        <v>0.42</v>
+        <v>0.21</v>
       </c>
       <c r="E58" t="n">
-        <v>24.74</v>
+        <v>21.77</v>
       </c>
       <c r="F58" t="n">
         <v>1.67</v>
       </c>
       <c r="G58" t="n">
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="H58" t="n">
-        <v>1.88</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="59">
@@ -6063,19 +6063,19 @@
         <v>10.69</v>
       </c>
       <c r="D59" t="n">
-        <v>2.63</v>
+        <v>3.3</v>
       </c>
       <c r="E59" t="n">
-        <v>12.18</v>
+        <v>16.33</v>
       </c>
       <c r="F59" t="n">
         <v>1.81</v>
       </c>
       <c r="G59" t="n">
-        <v>0.82</v>
+        <v>0.96</v>
       </c>
       <c r="H59" t="n">
-        <v>2.19</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="60">
@@ -6089,19 +6089,19 @@
         <v>832.19</v>
       </c>
       <c r="D60" t="n">
-        <v>27.26</v>
+        <v>33.05</v>
       </c>
       <c r="E60" t="n">
-        <v>851.15</v>
+        <v>941.35</v>
       </c>
       <c r="F60" t="n">
         <v>68.08</v>
       </c>
       <c r="G60" t="n">
-        <v>18.3</v>
+        <v>21.59</v>
       </c>
       <c r="H60" t="n">
-        <v>71.37</v>
+        <v>78.61</v>
       </c>
     </row>
     <row r="61">
@@ -6115,19 +6115,19 @@
         <v>205.54</v>
       </c>
       <c r="D61" t="n">
-        <v>22.78</v>
+        <v>34.5</v>
       </c>
       <c r="E61" t="n">
-        <v>274.54</v>
+        <v>341.7</v>
       </c>
       <c r="F61" t="n">
         <v>22.12</v>
       </c>
       <c r="G61" t="n">
-        <v>8.82</v>
+        <v>11.85</v>
       </c>
       <c r="H61" t="n">
-        <v>28.31</v>
+        <v>33.18</v>
       </c>
     </row>
     <row r="62">
@@ -6141,19 +6141,19 @@
         <v>66.1</v>
       </c>
       <c r="D62" t="n">
-        <v>33.58</v>
+        <v>17.51</v>
       </c>
       <c r="E62" t="n">
-        <v>20.94</v>
+        <v>46.22</v>
       </c>
       <c r="F62" t="n">
         <v>8.82</v>
       </c>
       <c r="G62" t="n">
-        <v>6.58</v>
+        <v>4.87</v>
       </c>
       <c r="H62" t="n">
-        <v>4.48</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="63">
@@ -6167,19 +6167,19 @@
         <v>83.88</v>
       </c>
       <c r="D63" t="n">
-        <v>147.34</v>
+        <v>74.79</v>
       </c>
       <c r="E63" t="n">
-        <v>73.87</v>
+        <v>45.82</v>
       </c>
       <c r="F63" t="n">
         <v>9.74</v>
       </c>
       <c r="G63" t="n">
-        <v>12.64</v>
+        <v>9.09</v>
       </c>
       <c r="H63" t="n">
-        <v>8.03</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="64">
@@ -6193,19 +6193,19 @@
         <v>1.15</v>
       </c>
       <c r="D64" t="n">
-        <v>31.88</v>
+        <v>36.7</v>
       </c>
       <c r="E64" t="n">
-        <v>43.2</v>
+        <v>48.73</v>
       </c>
       <c r="F64" t="n">
         <v>0.33</v>
       </c>
       <c r="G64" t="n">
-        <v>2.25</v>
+        <v>2.47</v>
       </c>
       <c r="H64" t="n">
-        <v>2.6</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="65">
@@ -6219,7 +6219,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1.93</v>
+        <v>2</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -6241,10 +6241,10 @@
         <v>0.01</v>
       </c>
       <c r="D66" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="E66" t="n">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F66" t="n">
         <v>0.01</v>
@@ -6267,19 +6267,19 @@
         <v>171.36</v>
       </c>
       <c r="D67" t="n">
-        <v>31.78</v>
+        <v>41.06</v>
       </c>
       <c r="E67" t="n">
-        <v>72.43</v>
+        <v>56.27</v>
       </c>
       <c r="F67" t="n">
         <v>8.53</v>
       </c>
       <c r="G67" t="n">
-        <v>4.29</v>
+        <v>4.84</v>
       </c>
       <c r="H67" t="n">
-        <v>4.49</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="68">
@@ -6293,19 +6293,19 @@
         <v>191.72</v>
       </c>
       <c r="D68" t="n">
-        <v>1.32</v>
+        <v>0.66</v>
       </c>
       <c r="E68" t="n">
-        <v>163.41</v>
+        <v>171.57</v>
       </c>
       <c r="F68" t="n">
         <v>12.77</v>
       </c>
       <c r="G68" t="n">
-        <v>0.66</v>
+        <v>0.53</v>
       </c>
       <c r="H68" t="n">
-        <v>11.98</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="69">
@@ -6319,19 +6319,19 @@
         <v>211.08</v>
       </c>
       <c r="D69" t="n">
-        <v>1.84</v>
+        <v>0.53</v>
       </c>
       <c r="E69" t="n">
-        <v>175.65</v>
+        <v>192.38</v>
       </c>
       <c r="F69" t="n">
         <v>13.17</v>
       </c>
       <c r="G69" t="n">
-        <v>0.79</v>
+        <v>0.4</v>
       </c>
       <c r="H69" t="n">
-        <v>12.38</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="70">
@@ -6345,19 +6345,19 @@
         <v>168.41</v>
       </c>
       <c r="D70" t="n">
-        <v>54.25</v>
+        <v>49.77</v>
       </c>
       <c r="E70" t="n">
-        <v>48.32</v>
+        <v>50.96</v>
       </c>
       <c r="F70" t="n">
         <v>11.98</v>
       </c>
       <c r="G70" t="n">
-        <v>5.66</v>
+        <v>5.4</v>
       </c>
       <c r="H70" t="n">
-        <v>6.32</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="71">
@@ -6371,19 +6371,19 @@
         <v>0.4</v>
       </c>
       <c r="D71" t="n">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="E71" t="n">
-        <v>0.19</v>
+        <v>0.77</v>
       </c>
       <c r="F71" t="n">
         <v>0.09</v>
       </c>
       <c r="G71" t="n">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="H71" t="n">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="72">
@@ -6397,14 +6397,14 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>71.35</v>
+        <v>62.91</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>33.38</v>
+        <v>32.34</v>
       </c>
       <c r="H72"/>
     </row>
@@ -6419,19 +6419,19 @@
         <v>95.46</v>
       </c>
       <c r="D73" t="n">
-        <v>17.73</v>
+        <v>17.8</v>
       </c>
       <c r="E73" t="n">
-        <v>191.96</v>
+        <v>192.18</v>
       </c>
       <c r="F73" t="n">
         <v>4.49</v>
       </c>
       <c r="G73" t="n">
-        <v>7.11</v>
+        <v>7.13</v>
       </c>
       <c r="H73" t="n">
-        <v>11.65</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="74">
@@ -6445,14 +6445,14 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>2.26</v>
+        <v>2.85</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>2.97</v>
+        <v>3.11</v>
       </c>
       <c r="H74"/>
     </row>
@@ -6474,7 +6474,7 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>2.42</v>
+        <v>2.41</v>
       </c>
       <c r="H75"/>
     </row>
@@ -6489,14 +6489,14 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>1.04</v>
+        <v>1.05</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>4.73</v>
+        <v>4.74</v>
       </c>
       <c r="H76"/>
     </row>
@@ -6511,14 +6511,14 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>367.47</v>
+        <v>363.82</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>121.81</v>
+        <v>119.82</v>
       </c>
       <c r="H77"/>
     </row>
@@ -6533,14 +6533,14 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.53</v>
+        <v>0.59</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>2.77</v>
+        <v>2.99</v>
       </c>
       <c r="H78"/>
     </row>
@@ -6555,14 +6555,14 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>10.81</v>
+        <v>10.72</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>40.97</v>
+        <v>40.75</v>
       </c>
       <c r="H79"/>
     </row>
@@ -6646,7 +6646,7 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H3"/>
     </row>
@@ -6727,10 +6727,10 @@
         <v>6.96</v>
       </c>
       <c r="D7" t="n">
-        <v>0.85</v>
+        <v>0.84</v>
       </c>
       <c r="E7" t="n">
-        <v>12.52</v>
+        <v>12.44</v>
       </c>
       <c r="F7" t="n">
         <v>0.71</v>
@@ -6756,13 +6756,13 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>17.57</v>
+        <v>17.48</v>
       </c>
       <c r="F8" t="n">
         <v>0.99</v>
       </c>
       <c r="G8" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H8" t="n">
         <v>0.99</v>
@@ -6782,7 +6782,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>17.8</v>
+        <v>17.79</v>
       </c>
       <c r="F9" t="n">
         <v>1</v>
@@ -6831,19 +6831,19 @@
         <v>13.52</v>
       </c>
       <c r="D11" t="n">
-        <v>0.26</v>
+        <v>0.16</v>
       </c>
       <c r="E11" t="n">
-        <v>17.05</v>
+        <v>16.35</v>
       </c>
       <c r="F11" t="n">
         <v>0.91</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09</v>
+        <v>0.07</v>
       </c>
       <c r="H11" t="n">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="12">
@@ -6860,16 +6860,16 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>13.65</v>
+        <v>14.04</v>
       </c>
       <c r="F12" t="n">
         <v>0.98</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="H12" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="13">
@@ -6886,7 +6886,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>15.45</v>
+        <v>15.44</v>
       </c>
       <c r="F13" t="n">
         <v>1</v>
@@ -6909,19 +6909,19 @@
         <v>11.56</v>
       </c>
       <c r="D14" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>10.44</v>
+        <v>11.59</v>
       </c>
       <c r="F14" t="n">
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0.96</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -6990,7 +6990,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>44.2</v>
+        <v>44.27</v>
       </c>
       <c r="F17" t="n">
         <v>3.74</v>
@@ -7013,19 +7013,19 @@
         <v>105.42</v>
       </c>
       <c r="D18" t="n">
-        <v>0.63</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>91.68</v>
+        <v>106.51</v>
       </c>
       <c r="F18" t="n">
         <v>9.04</v>
       </c>
       <c r="G18" t="n">
-        <v>0.36</v>
+        <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>8.59</v>
+        <v>9.04</v>
       </c>
     </row>
     <row r="19">
@@ -7039,19 +7039,19 @@
         <v>0.15</v>
       </c>
       <c r="D19" t="n">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="F19" t="n">
         <v>0.05</v>
       </c>
       <c r="G19" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="H19" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20">
@@ -7068,13 +7068,13 @@
         <v>0.11</v>
       </c>
       <c r="E20" t="n">
-        <v>179.8</v>
+        <v>177.66</v>
       </c>
       <c r="F20" t="n">
         <v>10.58</v>
       </c>
       <c r="G20" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="H20" t="n">
         <v>10.47</v>
@@ -7094,7 +7094,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>119.26</v>
+        <v>118.87</v>
       </c>
       <c r="F21" t="n">
         <v>7.72</v>
@@ -7120,7 +7120,7 @@
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>201.18</v>
+        <v>201.06</v>
       </c>
       <c r="F22" t="n">
         <v>12.29</v>
@@ -7143,19 +7143,19 @@
         <v>117.08</v>
       </c>
       <c r="D23" t="n">
-        <v>2.56</v>
+        <v>1.95</v>
       </c>
       <c r="E23" t="n">
-        <v>146.09</v>
+        <v>134.52</v>
       </c>
       <c r="F23" t="n">
         <v>11.42</v>
       </c>
       <c r="G23" t="n">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="H23" t="n">
-        <v>12.63</v>
+        <v>12.17</v>
       </c>
     </row>
     <row r="24">
@@ -7172,7 +7172,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>79.29</v>
+        <v>79.24</v>
       </c>
       <c r="F24" t="n">
         <v>5.11</v>
@@ -7195,19 +7195,19 @@
         <v>100.47</v>
       </c>
       <c r="D25" t="n">
-        <v>3.67</v>
+        <v>3.13</v>
       </c>
       <c r="E25" t="n">
-        <v>139.7</v>
+        <v>136.68</v>
       </c>
       <c r="F25" t="n">
         <v>8.95</v>
       </c>
       <c r="G25" t="n">
-        <v>1.08</v>
+        <v>0.97</v>
       </c>
       <c r="H25" t="n">
-        <v>10.13</v>
+        <v>10.02</v>
       </c>
     </row>
     <row r="26">
@@ -7250,7 +7250,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>268.18</v>
+        <v>267.87</v>
       </c>
       <c r="F27" t="n">
         <v>15.32</v>
@@ -7276,7 +7276,7 @@
         <v>0.22</v>
       </c>
       <c r="E28" t="n">
-        <v>365.63</v>
+        <v>364.74</v>
       </c>
       <c r="F28" t="n">
         <v>22.12</v>
@@ -7302,7 +7302,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>71.36</v>
+        <v>71.45</v>
       </c>
       <c r="F29" t="n">
         <v>4.58</v>
@@ -7325,19 +7325,19 @@
         <v>107.93</v>
       </c>
       <c r="D30" t="n">
-        <v>0.36</v>
+        <v>0.14</v>
       </c>
       <c r="E30" t="n">
-        <v>96.95</v>
+        <v>100.56</v>
       </c>
       <c r="F30" t="n">
         <v>7.23</v>
       </c>
       <c r="G30" t="n">
-        <v>0.29</v>
+        <v>0.14</v>
       </c>
       <c r="H30" t="n">
-        <v>7.01</v>
+        <v>7.08</v>
       </c>
     </row>
     <row r="31">
@@ -7377,19 +7377,19 @@
         <v>290.37</v>
       </c>
       <c r="D32" t="n">
-        <v>0.21</v>
+        <v>1.24</v>
       </c>
       <c r="E32" t="n">
-        <v>277.53</v>
+        <v>262.41</v>
       </c>
       <c r="F32" t="n">
         <v>20.5</v>
       </c>
       <c r="G32" t="n">
-        <v>0.41</v>
+        <v>0.83</v>
       </c>
       <c r="H32" t="n">
-        <v>20.09</v>
+        <v>19.68</v>
       </c>
     </row>
     <row r="33">
@@ -7451,19 +7451,19 @@
         <v>8.45</v>
       </c>
       <c r="D35" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>7.77</v>
+        <v>8.45</v>
       </c>
       <c r="F35" t="n">
         <v>0.99</v>
       </c>
       <c r="G35" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H35" t="n">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="36">
@@ -7503,10 +7503,10 @@
         <v>220.31</v>
       </c>
       <c r="D37" t="n">
-        <v>1.02</v>
+        <v>0.87</v>
       </c>
       <c r="E37" t="n">
-        <v>249.31</v>
+        <v>248.29</v>
       </c>
       <c r="F37" t="n">
         <v>13.7</v>
@@ -7529,19 +7529,19 @@
         <v>218.1</v>
       </c>
       <c r="D38" t="n">
-        <v>0.53</v>
+        <v>0.13</v>
       </c>
       <c r="E38" t="n">
-        <v>204.43</v>
+        <v>215.72</v>
       </c>
       <c r="F38" t="n">
         <v>12.61</v>
       </c>
       <c r="G38" t="n">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="H38" t="n">
-        <v>12.48</v>
+        <v>12.61</v>
       </c>
     </row>
     <row r="39">
@@ -7555,10 +7555,10 @@
         <v>164.3</v>
       </c>
       <c r="D39" t="n">
-        <v>37.9</v>
+        <v>35.99</v>
       </c>
       <c r="E39" t="n">
-        <v>345.32</v>
+        <v>341.93</v>
       </c>
       <c r="F39" t="n">
         <v>15.24</v>
@@ -7567,7 +7567,7 @@
         <v>5.29</v>
       </c>
       <c r="H39" t="n">
-        <v>20.54</v>
+        <v>20.33</v>
       </c>
     </row>
     <row r="40">
@@ -7584,7 +7584,7 @@
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>203.31</v>
+        <v>201.99</v>
       </c>
       <c r="F40" t="n">
         <v>13.17</v>
@@ -7633,7 +7633,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>0.51</v>
+        <v>0.48</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
@@ -7655,16 +7655,16 @@
         <v>0.06</v>
       </c>
       <c r="D43" t="n">
-        <v>0.67</v>
+        <v>0.78</v>
       </c>
       <c r="E43" t="n">
-        <v>0.61</v>
+        <v>0.72</v>
       </c>
       <c r="F43" t="n">
         <v>0.06</v>
       </c>
       <c r="G43" t="n">
-        <v>0.28</v>
+        <v>0.33</v>
       </c>
       <c r="H43" t="n">
         <v>0.28</v>
@@ -7681,19 +7681,19 @@
         <v>11.32</v>
       </c>
       <c r="D44" t="n">
-        <v>10.31</v>
+        <v>9.82</v>
       </c>
       <c r="E44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
       <c r="F44" t="n">
         <v>1.21</v>
       </c>
       <c r="G44" t="n">
-        <v>1.15</v>
+        <v>1.11</v>
       </c>
       <c r="H44" t="n">
-        <v>0.07</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="45">
@@ -7707,7 +7707,7 @@
         <v>0.14</v>
       </c>
       <c r="D45" t="n">
-        <v>0.86</v>
+        <v>0.72</v>
       </c>
       <c r="E45" t="n">
         <v>0.57</v>
@@ -7733,19 +7733,19 @@
         <v>0.15</v>
       </c>
       <c r="D46" t="n">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F46" t="n">
         <v>0.12</v>
       </c>
       <c r="G46" t="n">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="H46" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="47">
@@ -7759,19 +7759,19 @@
         <v>0.18</v>
       </c>
       <c r="D47" t="n">
-        <v>3.32</v>
+        <v>3.78</v>
       </c>
       <c r="E47" t="n">
-        <v>4.43</v>
+        <v>4.98</v>
       </c>
       <c r="F47" t="n">
         <v>0.18</v>
       </c>
       <c r="G47" t="n">
-        <v>1.01</v>
+        <v>1.11</v>
       </c>
       <c r="H47" t="n">
-        <v>1.2</v>
+        <v>1.29</v>
       </c>
     </row>
     <row r="48">
@@ -7785,7 +7785,7 @@
         <v>1.62</v>
       </c>
       <c r="D48" t="n">
-        <v>0.81</v>
+        <v>0.86</v>
       </c>
       <c r="E48" t="n">
         <v>2.48</v>
@@ -7811,19 +7811,19 @@
         <v>3.05</v>
       </c>
       <c r="D49" t="n">
-        <v>0.05</v>
+        <v>0.22</v>
       </c>
       <c r="E49" t="n">
-        <v>2.9</v>
+        <v>2.15</v>
       </c>
       <c r="F49" t="n">
         <v>0.82</v>
       </c>
       <c r="G49" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="H49" t="n">
-        <v>0.8</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="50">
@@ -7837,19 +7837,19 @@
         <v>2403.09</v>
       </c>
       <c r="D50" t="n">
-        <v>2385.13</v>
+        <v>2312.93</v>
       </c>
       <c r="E50" t="n">
-        <v>2.5</v>
+        <v>6.48</v>
       </c>
       <c r="F50" t="n">
         <v>128.7</v>
       </c>
       <c r="G50" t="n">
-        <v>127.68</v>
+        <v>127.23</v>
       </c>
       <c r="H50" t="n">
-        <v>0.91</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="51">
@@ -7866,7 +7866,7 @@
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>52.9</v>
+        <v>52.75</v>
       </c>
       <c r="F51" t="n">
         <v>3.64</v>
@@ -7875,7 +7875,7 @@
         <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>3.64</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="52">
@@ -7889,19 +7889,19 @@
         <v>84.79</v>
       </c>
       <c r="D52" t="n">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="E52" t="n">
-        <v>80.48</v>
+        <v>85.77</v>
       </c>
       <c r="F52" t="n">
         <v>5.51</v>
       </c>
       <c r="G52" t="n">
-        <v>0.11</v>
+        <v>0.06</v>
       </c>
       <c r="H52" t="n">
-        <v>5.4</v>
+        <v>5.51</v>
       </c>
     </row>
     <row r="53">
@@ -7915,19 +7915,19 @@
         <v>2.91</v>
       </c>
       <c r="D53" t="n">
-        <v>0.1</v>
+        <v>0.31</v>
       </c>
       <c r="E53" t="n">
-        <v>3.53</v>
+        <v>4.47</v>
       </c>
       <c r="F53" t="n">
         <v>1.04</v>
       </c>
       <c r="G53" t="n">
-        <v>0.1</v>
+        <v>0.21</v>
       </c>
       <c r="H53" t="n">
-        <v>1.14</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="54">
@@ -7941,14 +7941,14 @@
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="E54" t="n">
         <v>0</v>
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H54"/>
     </row>
@@ -7963,14 +7963,14 @@
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="E55" t="n">
         <v>0</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="H55"/>
     </row>
@@ -8007,14 +8007,14 @@
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="H57"/>
     </row>
@@ -8029,19 +8029,19 @@
         <v>27.1</v>
       </c>
       <c r="D58" t="n">
-        <v>0.24</v>
+        <v>0.45</v>
       </c>
       <c r="E58" t="n">
-        <v>24.74</v>
+        <v>21.77</v>
       </c>
       <c r="F58" t="n">
         <v>2</v>
       </c>
       <c r="G58" t="n">
-        <v>0.18</v>
+        <v>0.27</v>
       </c>
       <c r="H58" t="n">
-        <v>1.88</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="59">
@@ -8055,19 +8055,19 @@
         <v>4.84</v>
       </c>
       <c r="D59" t="n">
-        <v>4.84</v>
+        <v>6.91</v>
       </c>
       <c r="E59" t="n">
-        <v>12.18</v>
+        <v>16.33</v>
       </c>
       <c r="F59" t="n">
         <v>1.02</v>
       </c>
       <c r="G59" t="n">
-        <v>0.98</v>
+        <v>1.26</v>
       </c>
       <c r="H59" t="n">
-        <v>2.19</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="60">
@@ -8081,19 +8081,19 @@
         <v>477.32</v>
       </c>
       <c r="D60" t="n">
-        <v>83.09</v>
+        <v>110.48</v>
       </c>
       <c r="E60" t="n">
-        <v>851.15</v>
+        <v>941.35</v>
       </c>
       <c r="F60" t="n">
         <v>42.14</v>
       </c>
       <c r="G60" t="n">
-        <v>29.63</v>
+        <v>36.47</v>
       </c>
       <c r="H60" t="n">
-        <v>71.37</v>
+        <v>78.61</v>
       </c>
     </row>
     <row r="61">
@@ -8107,19 +8107,19 @@
         <v>108.37</v>
       </c>
       <c r="D61" t="n">
-        <v>62.68</v>
+        <v>90.46</v>
       </c>
       <c r="E61" t="n">
-        <v>274.54</v>
+        <v>341.7</v>
       </c>
       <c r="F61" t="n">
         <v>13.56</v>
       </c>
       <c r="G61" t="n">
-        <v>14.75</v>
+        <v>19.62</v>
       </c>
       <c r="H61" t="n">
-        <v>28.31</v>
+        <v>33.18</v>
       </c>
     </row>
     <row r="62">
@@ -8133,19 +8133,19 @@
         <v>46.22</v>
       </c>
       <c r="D62" t="n">
-        <v>19.09</v>
+        <v>22.38</v>
       </c>
       <c r="E62" t="n">
-        <v>20.94</v>
+        <v>46.22</v>
       </c>
       <c r="F62" t="n">
         <v>6.85</v>
       </c>
       <c r="G62" t="n">
-        <v>4.74</v>
+        <v>5.14</v>
       </c>
       <c r="H62" t="n">
-        <v>4.48</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="63">
@@ -8159,19 +8159,19 @@
         <v>66.76</v>
       </c>
       <c r="D63" t="n">
-        <v>89.41</v>
+        <v>41.87</v>
       </c>
       <c r="E63" t="n">
-        <v>73.87</v>
+        <v>45.82</v>
       </c>
       <c r="F63" t="n">
         <v>8.3</v>
       </c>
       <c r="G63" t="n">
-        <v>8.82</v>
+        <v>6.06</v>
       </c>
       <c r="H63" t="n">
-        <v>8.03</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="64">
@@ -8185,19 +8185,19 @@
         <v>12.31</v>
       </c>
       <c r="D64" t="n">
-        <v>11.16</v>
+        <v>14.31</v>
       </c>
       <c r="E64" t="n">
-        <v>43.2</v>
+        <v>48.73</v>
       </c>
       <c r="F64" t="n">
         <v>1.18</v>
       </c>
       <c r="G64" t="n">
-        <v>1.4</v>
+        <v>1.62</v>
       </c>
       <c r="H64" t="n">
-        <v>2.6</v>
+        <v>2.85</v>
       </c>
     </row>
     <row r="65">
@@ -8211,7 +8211,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1.62</v>
+        <v>1.69</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -8233,16 +8233,16 @@
         <v>0.01</v>
       </c>
       <c r="D66" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="E66" t="n">
         <v>0.16</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.17</v>
       </c>
       <c r="F66" t="n">
         <v>0.01</v>
       </c>
       <c r="G66" t="n">
-        <v>0.09</v>
+        <v>0.07</v>
       </c>
       <c r="H66" t="n">
         <v>0.09</v>
@@ -8259,19 +8259,19 @@
         <v>290.33</v>
       </c>
       <c r="D67" t="n">
-        <v>88.05</v>
+        <v>105.31</v>
       </c>
       <c r="E67" t="n">
-        <v>72.43</v>
+        <v>56.27</v>
       </c>
       <c r="F67" t="n">
         <v>13.22</v>
       </c>
       <c r="G67" t="n">
-        <v>8.73</v>
+        <v>9.43</v>
       </c>
       <c r="H67" t="n">
-        <v>4.49</v>
+        <v>3.79</v>
       </c>
     </row>
     <row r="68">
@@ -8285,19 +8285,19 @@
         <v>207.26</v>
       </c>
       <c r="D68" t="n">
-        <v>3.03</v>
+        <v>1.98</v>
       </c>
       <c r="E68" t="n">
-        <v>163.41</v>
+        <v>171.57</v>
       </c>
       <c r="F68" t="n">
         <v>13.17</v>
       </c>
       <c r="G68" t="n">
-        <v>1.05</v>
+        <v>0.79</v>
       </c>
       <c r="H68" t="n">
-        <v>11.98</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="69">
@@ -8311,19 +8311,19 @@
         <v>210.94</v>
       </c>
       <c r="D69" t="n">
-        <v>1.84</v>
+        <v>0.53</v>
       </c>
       <c r="E69" t="n">
-        <v>175.65</v>
+        <v>192.38</v>
       </c>
       <c r="F69" t="n">
         <v>13.17</v>
       </c>
       <c r="G69" t="n">
-        <v>0.79</v>
+        <v>0.4</v>
       </c>
       <c r="H69" t="n">
-        <v>12.38</v>
+        <v>12.77</v>
       </c>
     </row>
     <row r="70">
@@ -8337,19 +8337,19 @@
         <v>161.17</v>
       </c>
       <c r="D70" t="n">
-        <v>49.51</v>
+        <v>45.3</v>
       </c>
       <c r="E70" t="n">
-        <v>48.32</v>
+        <v>50.96</v>
       </c>
       <c r="F70" t="n">
         <v>11.72</v>
       </c>
       <c r="G70" t="n">
-        <v>5.4</v>
+        <v>5.14</v>
       </c>
       <c r="H70" t="n">
-        <v>6.32</v>
+        <v>6.58</v>
       </c>
     </row>
     <row r="71">
@@ -8363,19 +8363,19 @@
         <v>0.33</v>
       </c>
       <c r="D71" t="n">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="E71" t="n">
-        <v>0.19</v>
+        <v>0.77</v>
       </c>
       <c r="F71" t="n">
         <v>0.08</v>
       </c>
       <c r="G71" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="H71" t="n">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="72">
@@ -8389,14 +8389,14 @@
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>43.76</v>
+        <v>37.35</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>20.3</v>
+        <v>19.26</v>
       </c>
       <c r="H72"/>
     </row>
@@ -8411,19 +8411,19 @@
         <v>100.64</v>
       </c>
       <c r="D73" t="n">
-        <v>15.49</v>
+        <v>15.55</v>
       </c>
       <c r="E73" t="n">
-        <v>191.96</v>
+        <v>192.18</v>
       </c>
       <c r="F73" t="n">
         <v>4.78</v>
       </c>
       <c r="G73" t="n">
-        <v>6.81</v>
+        <v>6.84</v>
       </c>
       <c r="H73" t="n">
-        <v>11.65</v>
+        <v>11.67</v>
       </c>
     </row>
     <row r="74">
@@ -8437,14 +8437,14 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>3.87</v>
+        <v>6.18</v>
       </c>
       <c r="E74" t="n">
         <v>0</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>3.82</v>
+        <v>4.78</v>
       </c>
       <c r="H74"/>
     </row>
@@ -8459,14 +8459,14 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>0.28</v>
+        <v>0.29</v>
       </c>
       <c r="E75" t="n">
         <v>0</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>1.42</v>
+        <v>1.43</v>
       </c>
       <c r="H75"/>
     </row>
@@ -8481,7 +8481,7 @@
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>2.45</v>
+        <v>2.46</v>
       </c>
       <c r="E76" t="n">
         <v>0</v>
@@ -8503,14 +8503,14 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>386.52</v>
+        <v>382.77</v>
       </c>
       <c r="E77" t="n">
         <v>0</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>122.23</v>
+        <v>120.24</v>
       </c>
       <c r="H77"/>
     </row>
@@ -8525,14 +8525,14 @@
         <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>0.63</v>
+        <v>0.61</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>2.87</v>
+        <v>2.77</v>
       </c>
       <c r="H78"/>
     </row>
@@ -8547,14 +8547,14 @@
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>6.41</v>
+        <v>6.34</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>33.19</v>
+        <v>32.98</v>
       </c>
       <c r="H79"/>
     </row>

</xml_diff>